<commit_message>
update chart & logbook
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Project</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Day 1</t>
   </si>
   <si>
-    <t>Story 1</t>
-  </si>
-  <si>
     <t>Story 2</t>
   </si>
   <si>
@@ -118,15 +115,6 @@
   </si>
   <si>
     <t>Story 4</t>
-  </si>
-  <si>
-    <t>Task 1.1</t>
-  </si>
-  <si>
-    <t>Task 1.2</t>
-  </si>
-  <si>
-    <t>Task 1.3</t>
   </si>
   <si>
     <t>Task 2.1</t>
@@ -172,6 +160,24 @@
   </si>
   <si>
     <t>Android</t>
+  </si>
+  <si>
+    <t>Pengenalan Android</t>
+  </si>
+  <si>
+    <t>Apa itut Android ?</t>
+  </si>
+  <si>
+    <t>Sedikit Sejarah Android</t>
+  </si>
+  <si>
+    <t>Jelaskan ICS</t>
+  </si>
+  <si>
+    <t>Jelaskan JB</t>
+  </si>
+  <si>
+    <t>Jelaskan Kitkat</t>
   </si>
 </sst>
 </file>
@@ -386,36 +392,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$O$19</c:f>
+              <c:f>Sheet1!$F$21:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>81</c:v>
+                  <c:v>72.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72</c:v>
+                  <c:v>64.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63</c:v>
+                  <c:v>56.70000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>48.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45</c:v>
+                  <c:v>40.500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>32.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>24.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>16.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>8.1000000000000032</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -473,7 +479,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$20:$O$20</c:f>
+              <c:f>Sheet1!$F$22:$O$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -500,25 +506,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="94747648"/>
-        <c:axId val="141980416"/>
+        <c:axId val="91753472"/>
+        <c:axId val="145593088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94747648"/>
+        <c:axId val="91753472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141980416"/>
+        <c:crossAx val="145593088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141980416"/>
+        <c:axId val="145593088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +532,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="94747648"/>
+        <c:crossAx val="91753472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -539,7 +545,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -551,13 +557,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -865,17 +871,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD56"/>
+  <dimension ref="A1:XFD58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" s="5" customFormat="1" ht="15.75">
@@ -884,7 +890,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -33657,7 +33663,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -50113,16 +50119,16 @@
     <row r="6" spans="1:16384">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E6" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4">
         <v>4</v>
@@ -50152,16 +50158,16 @@
     <row r="7" spans="1:16384">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7" s="4">
         <v>2</v>
@@ -50191,32 +50197,22 @@
     <row r="8" spans="1:16384">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" s="4">
-        <v>5</v>
-      </c>
-      <c r="F8" s="4">
-        <v>5</v>
-      </c>
-      <c r="G8" s="4">
-        <v>3</v>
-      </c>
-      <c r="H8" s="4">
         <v>2</v>
       </c>
-      <c r="I8" s="4">
-        <v>2</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -50230,32 +50226,22 @@
     <row r="9" spans="1:16384">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E9" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
-      <c r="F9" s="4">
-        <v>8</v>
-      </c>
-      <c r="G9" s="4">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4">
-        <v>8</v>
-      </c>
-      <c r="I9" s="4">
-        <v>7</v>
-      </c>
-      <c r="J9" s="4">
-        <v>3</v>
-      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -50269,31 +50255,31 @@
     <row r="10" spans="1:16384">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E10" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F10" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G10" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H10" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I10" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J10" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -50308,31 +50294,31 @@
     <row r="11" spans="1:16384">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E11" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J11" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -50347,31 +50333,31 @@
     <row r="12" spans="1:16384">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J12" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -50386,31 +50372,31 @@
     <row r="13" spans="1:16384">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E13" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F13" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G13" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H13" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I13" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J13" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -50425,31 +50411,31 @@
     <row r="14" spans="1:16384">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E14" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G14" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H14" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I14" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J14" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -50464,31 +50450,31 @@
     <row r="15" spans="1:16384">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E15" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I15" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J15" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -50503,31 +50489,31 @@
     <row r="16" spans="1:16384">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E16" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F16" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G16" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H16" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I16" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J16" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -50542,13 +50528,13 @@
     <row r="17" spans="1:19">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E17" s="4">
         <v>8</v>
@@ -50581,31 +50567,31 @@
     <row r="18" spans="1:19">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E18" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F18" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G18" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H18" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I18" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J18" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -50619,55 +50605,38 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="1"/>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E19" s="4">
-        <f>SUM(E6:E18)</f>
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="F19" s="4">
-        <f>E19-$E$19/10</f>
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" ref="G19:O19" si="0">F19-$E$19/10</f>
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <v>8</v>
       </c>
-      <c r="K19" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="M19" s="4">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="N19" s="4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="O19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -50675,34 +50644,32 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="1"/>
-      <c r="B20" s="7" t="s">
-        <v>32</v>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E20" s="4">
-        <f>SUM(E6:E18)</f>
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" ref="F20:J20" si="1">SUM(F6:F18)</f>
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="1"/>
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="1"/>
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="1"/>
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="1"/>
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -50716,20 +50683,55 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="B21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="4">
+        <f>SUM(E6:E20)</f>
+        <v>81</v>
+      </c>
+      <c r="F21" s="4">
+        <f>E21-$E$21/10</f>
+        <v>72.900000000000006</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" ref="G21:O21" si="0">F21-$E$21/10</f>
+        <v>64.800000000000011</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>56.70000000000001</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
+        <v>48.600000000000009</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="0"/>
+        <v>40.500000000000007</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="0"/>
+        <v>24.300000000000004</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="0"/>
+        <v>16.200000000000003</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="0"/>
+        <v>8.1000000000000032</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -50737,20 +50739,40 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="B22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="4">
+        <f>SUM(E6:E20)</f>
+        <v>81</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" ref="F22:J22" si="1">SUM(F6:F20)</f>
+        <v>82</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -51470,11 +51492,53 @@
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
     </row>
+    <row r="57" spans="1:19">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+    </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="E1:H1"/>
   </mergeCells>

</xml_diff>

<commit_message>
update logbook day 2
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -21,7 +21,7 @@
     <author>mkg</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Project</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>Jelaskan Kitkat</t>
+  </si>
+  <si>
+    <t>Day 11</t>
+  </si>
+  <si>
+    <t>Day 12</t>
   </si>
 </sst>
 </file>
@@ -354,7 +360,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$5:$O$5</c:f>
+              <c:f>Sheet1!$H$5:$Q$5</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -392,7 +398,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$21:$O$21</c:f>
+              <c:f>Sheet1!$H$21:$Q$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -441,7 +447,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$5:$O$5</c:f>
+              <c:f>Sheet1!$H$5:$Q$5</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -479,7 +485,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$O$22</c:f>
+              <c:f>Sheet1!$H$22:$Q$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -506,25 +512,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="91753472"/>
-        <c:axId val="145593088"/>
+        <c:axId val="98229248"/>
+        <c:axId val="137921280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91753472"/>
+        <c:axId val="98229248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145593088"/>
+        <c:crossAx val="137921280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145593088"/>
+        <c:axId val="137921280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,7 +538,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="91753472"/>
+        <c:crossAx val="98229248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -545,7 +551,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -561,7 +567,7 @@
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
@@ -873,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -895,8 +901,8 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -33670,8 +33676,8 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -50066,6 +50072,8 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:16384">
       <c r="A5" s="1"/>
@@ -50082,39 +50090,45 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" s="1"/>
@@ -50130,14 +50144,10 @@
       <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
         <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
@@ -50145,15 +50155,21 @@
       <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:16384">
       <c r="A7" s="1"/>
@@ -50169,30 +50185,32 @@
       <c r="E7" s="4">
         <v>2</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
         <v>2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="I7" s="4">
         <v>3</v>
       </c>
-      <c r="H7" s="4">
+      <c r="J7" s="4">
         <v>5</v>
       </c>
-      <c r="I7" s="4">
+      <c r="K7" s="4">
         <v>2</v>
       </c>
-      <c r="J7" s="4">
+      <c r="L7" s="4">
         <v>0</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:16384">
       <c r="A8" s="1"/>
@@ -50218,10 +50236,12 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:16384">
       <c r="A9" s="1"/>
@@ -50247,10 +50267,12 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
     </row>
     <row r="10" spans="1:16384">
       <c r="A10" s="1"/>
@@ -50266,30 +50288,32 @@
       <c r="E10" s="4">
         <v>2</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
         <v>5</v>
       </c>
-      <c r="G10" s="4">
+      <c r="I10" s="4">
         <v>3</v>
       </c>
-      <c r="H10" s="4">
+      <c r="J10" s="4">
         <v>2</v>
       </c>
-      <c r="I10" s="4">
+      <c r="K10" s="4">
         <v>2</v>
       </c>
-      <c r="J10" s="4">
+      <c r="L10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
     </row>
     <row r="11" spans="1:16384">
       <c r="A11" s="1"/>
@@ -50305,30 +50329,32 @@
       <c r="E11" s="4">
         <v>8</v>
       </c>
-      <c r="F11" s="4">
-        <v>8</v>
-      </c>
-      <c r="G11" s="4">
-        <v>8</v>
-      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="4">
         <v>8</v>
       </c>
       <c r="I11" s="4">
+        <v>8</v>
+      </c>
+      <c r="J11" s="4">
+        <v>8</v>
+      </c>
+      <c r="K11" s="4">
         <v>7</v>
       </c>
-      <c r="J11" s="4">
+      <c r="L11" s="4">
         <v>3</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
     </row>
     <row r="12" spans="1:16384">
       <c r="A12" s="1"/>
@@ -50344,12 +50370,8 @@
       <c r="E12" s="4">
         <v>8</v>
       </c>
-      <c r="F12" s="4">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4">
-        <v>8</v>
-      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="4">
         <v>8</v>
       </c>
@@ -50357,17 +50379,23 @@
         <v>8</v>
       </c>
       <c r="J12" s="4">
+        <v>8</v>
+      </c>
+      <c r="K12" s="4">
+        <v>8</v>
+      </c>
+      <c r="L12" s="4">
         <v>7</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
     </row>
     <row r="13" spans="1:16384">
       <c r="A13" s="1"/>
@@ -50383,12 +50411,8 @@
       <c r="E13" s="4">
         <v>9</v>
       </c>
-      <c r="F13" s="4">
-        <v>9</v>
-      </c>
-      <c r="G13" s="4">
-        <v>9</v>
-      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="4">
         <v>9</v>
       </c>
@@ -50398,15 +50422,21 @@
       <c r="J13" s="4">
         <v>9</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="K13" s="4">
+        <v>9</v>
+      </c>
+      <c r="L13" s="4">
+        <v>9</v>
+      </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
     </row>
     <row r="14" spans="1:16384">
       <c r="A14" s="1"/>
@@ -50422,12 +50452,8 @@
       <c r="E14" s="4">
         <v>5</v>
       </c>
-      <c r="F14" s="4">
-        <v>5</v>
-      </c>
-      <c r="G14" s="4">
-        <v>5</v>
-      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="4">
         <v>5</v>
       </c>
@@ -50437,15 +50463,21 @@
       <c r="J14" s="4">
         <v>5</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="K14" s="4">
+        <v>5</v>
+      </c>
+      <c r="L14" s="4">
+        <v>5</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:16384">
       <c r="A15" s="1"/>
@@ -50461,12 +50493,8 @@
       <c r="E15" s="4">
         <v>7</v>
       </c>
-      <c r="F15" s="4">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4">
-        <v>7</v>
-      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="4">
         <v>7</v>
       </c>
@@ -50476,15 +50504,21 @@
       <c r="J15" s="4">
         <v>7</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="K15" s="4">
+        <v>7</v>
+      </c>
+      <c r="L15" s="4">
+        <v>7</v>
+      </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
     </row>
     <row r="16" spans="1:16384">
       <c r="A16" s="1"/>
@@ -50500,12 +50534,8 @@
       <c r="E16" s="4">
         <v>3</v>
       </c>
-      <c r="F16" s="4">
-        <v>3</v>
-      </c>
-      <c r="G16" s="4">
-        <v>3</v>
-      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="4">
         <v>3</v>
       </c>
@@ -50515,17 +50545,23 @@
       <c r="J16" s="4">
         <v>3</v>
       </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="K16" s="4">
+        <v>3</v>
+      </c>
+      <c r="L16" s="4">
+        <v>3</v>
+      </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
         <v>31</v>
@@ -50539,12 +50575,8 @@
       <c r="E17" s="4">
         <v>8</v>
       </c>
-      <c r="F17" s="4">
-        <v>8</v>
-      </c>
-      <c r="G17" s="4">
-        <v>8</v>
-      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="4">
         <v>8</v>
       </c>
@@ -50554,17 +50586,23 @@
       <c r="J17" s="4">
         <v>8</v>
       </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="K17" s="4">
+        <v>8</v>
+      </c>
+      <c r="L17" s="4">
+        <v>8</v>
+      </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:21">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
         <v>31</v>
@@ -50578,12 +50616,8 @@
       <c r="E18" s="4">
         <v>6</v>
       </c>
-      <c r="F18" s="4">
-        <v>6</v>
-      </c>
-      <c r="G18" s="4">
-        <v>6</v>
-      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
       <c r="H18" s="4">
         <v>6</v>
       </c>
@@ -50593,17 +50627,23 @@
       <c r="J18" s="4">
         <v>6</v>
       </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="K18" s="4">
+        <v>6</v>
+      </c>
+      <c r="L18" s="4">
+        <v>6</v>
+      </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
         <v>31</v>
@@ -50617,12 +50657,8 @@
       <c r="E19" s="4">
         <v>8</v>
       </c>
-      <c r="F19" s="4">
-        <v>8</v>
-      </c>
-      <c r="G19" s="4">
-        <v>8</v>
-      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
       <c r="H19" s="4">
         <v>8</v>
       </c>
@@ -50632,17 +50668,23 @@
       <c r="J19" s="4">
         <v>8</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+      <c r="K19" s="4">
+        <v>8</v>
+      </c>
+      <c r="L19" s="4">
+        <v>8</v>
+      </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
         <v>31</v>
@@ -50656,12 +50698,8 @@
       <c r="E20" s="4">
         <v>9</v>
       </c>
-      <c r="F20" s="4">
-        <v>9</v>
-      </c>
-      <c r="G20" s="4">
-        <v>9</v>
-      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
       <c r="H20" s="4">
         <v>9</v>
       </c>
@@ -50671,17 +50709,23 @@
       <c r="J20" s="4">
         <v>9</v>
       </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="K20" s="4">
+        <v>9</v>
+      </c>
+      <c r="L20" s="4">
+        <v>9</v>
+      </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
         <v>27</v>
@@ -50692,52 +50736,54 @@
         <f>SUM(E6:E20)</f>
         <v>81</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4">
         <f>E21-$E$21/10</f>
         <v>72.900000000000006</v>
       </c>
-      <c r="G21" s="4">
-        <f t="shared" ref="G21:O21" si="0">F21-$E$21/10</f>
+      <c r="I21" s="4">
+        <f t="shared" ref="I21:Q21" si="0">H21-$E$21/10</f>
         <v>64.800000000000011</v>
       </c>
-      <c r="H21" s="4">
+      <c r="J21" s="4">
         <f t="shared" si="0"/>
         <v>56.70000000000001</v>
       </c>
-      <c r="I21" s="4">
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
         <v>48.600000000000009</v>
       </c>
-      <c r="J21" s="4">
+      <c r="L21" s="4">
         <f t="shared" si="0"/>
         <v>40.500000000000007</v>
       </c>
-      <c r="K21" s="4">
+      <c r="M21" s="4">
         <f t="shared" si="0"/>
         <v>32.400000000000006</v>
       </c>
-      <c r="L21" s="4">
+      <c r="N21" s="4">
         <f t="shared" si="0"/>
         <v>24.300000000000004</v>
       </c>
-      <c r="M21" s="4">
+      <c r="O21" s="4">
         <f t="shared" si="0"/>
         <v>16.200000000000003</v>
       </c>
-      <c r="N21" s="4">
+      <c r="P21" s="4">
         <f t="shared" si="0"/>
         <v>8.1000000000000032</v>
       </c>
-      <c r="O21" s="4">
+      <c r="Q21" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="s">
         <v>28</v>
@@ -50748,37 +50794,39 @@
         <f>SUM(E6:E20)</f>
         <v>81</v>
       </c>
-      <c r="F22" s="4">
-        <f t="shared" ref="F22:J22" si="1">SUM(F6:F20)</f>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
+        <f t="shared" ref="H22:L22" si="1">SUM(H6:H20)</f>
         <v>82</v>
       </c>
-      <c r="G22" s="4">
+      <c r="I22" s="4">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="H22" s="4">
+      <c r="J22" s="4">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="I22" s="4">
+      <c r="K22" s="4">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="J22" s="4">
+      <c r="L22" s="4">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:21">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -50798,8 +50846,10 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:21">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -50819,8 +50869,10 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:21">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -50840,8 +50892,10 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:21">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -50861,8 +50915,10 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:21">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -50882,8 +50938,10 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:21">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -50903,8 +50961,10 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:21">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -50924,8 +50984,10 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:21">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -50945,8 +51007,10 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:21">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -50966,8 +51030,10 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:21">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -50987,8 +51053,10 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:21">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -51008,8 +51076,10 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:21">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -51029,8 +51099,10 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:21">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -51050,8 +51122,10 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:21">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -51071,8 +51145,10 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:21">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -51092,8 +51168,10 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:21">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -51113,8 +51191,10 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:21">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -51134,8 +51214,10 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:21">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -51155,8 +51237,10 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:21">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -51176,8 +51260,10 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:21">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -51197,8 +51283,10 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:21">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -51218,8 +51306,10 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:21">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -51239,8 +51329,10 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:21">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -51260,8 +51352,10 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:21">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -51281,8 +51375,10 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:21">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -51302,8 +51398,10 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:21">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -51323,8 +51421,10 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:21">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -51344,8 +51444,10 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:21">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -51365,8 +51467,10 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:21">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -51386,8 +51490,10 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:21">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -51407,8 +51513,10 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:21">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -51428,8 +51536,10 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:21">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -51449,8 +51559,10 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:21">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -51470,8 +51582,10 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:21">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -51491,8 +51605,10 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:21">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -51512,8 +51628,10 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:21">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -51533,14 +51651,16 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
     </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="E1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit BurnDownChart & LogBook
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -186,7 +186,7 @@
     <t>Benchmark Apps</t>
   </si>
   <si>
-    <t>Re-design tampilan</t>
+    <t>Kegunaan Benchmark</t>
   </si>
 </sst>
 </file>
@@ -412,37 +412,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>71.5</c:v>
+                  <c:v>64.166666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>58.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58.5</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52</c:v>
+                  <c:v>46.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.5</c:v>
+                  <c:v>40.833333333333329</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>34.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.5</c:v>
+                  <c:v>29.166666666666661</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>23.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.5</c:v>
+                  <c:v>17.499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>11.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.5</c:v>
+                  <c:v>5.8333333333333313</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -511,13 +511,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -533,25 +533,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="211817600"/>
-        <c:axId val="211819136"/>
+        <c:axId val="58211328"/>
+        <c:axId val="60351232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="211817600"/>
+        <c:axId val="58211328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211819136"/>
+        <c:crossAx val="60351232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211819136"/>
+        <c:axId val="60351232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +559,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211817600"/>
+        <c:crossAx val="58211328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -572,7 +572,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50491,22 +50491,22 @@
         <v>35</v>
       </c>
       <c r="E14" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F14" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G14" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H14" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I14" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J14" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -50532,22 +50532,22 @@
         <v>36</v>
       </c>
       <c r="E15" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G15" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H15" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I15" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J15" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -50573,22 +50573,22 @@
         <v>38</v>
       </c>
       <c r="E16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -50611,25 +50611,25 @@
         <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F17" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G17" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H17" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I17" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J17" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
@@ -50652,7 +50652,7 @@
         <v>37</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4">
         <v>10</v>
@@ -50775,51 +50775,51 @@
       <c r="D21" s="7"/>
       <c r="E21" s="4">
         <f>SUM(E6:E20)</f>
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F21" s="4">
         <f>E21-$E$21/12</f>
-        <v>71.5</v>
+        <v>64.166666666666671</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" ref="G21:Q21" si="0">F21-$E$21/12</f>
-        <v>65</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="0"/>
-        <v>58.5</v>
+        <v>52.5</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>46.666666666666664</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="0"/>
-        <v>45.5</v>
+        <v>40.833333333333329</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>34.999999999999993</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="0"/>
-        <v>32.5</v>
+        <v>29.166666666666661</v>
       </c>
       <c r="M21" s="4">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>23.333333333333329</v>
       </c>
       <c r="N21" s="4">
         <f>M21-$E$21/12</f>
-        <v>19.5</v>
+        <v>17.499999999999996</v>
       </c>
       <c r="O21" s="4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11.666666666666664</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>5.8333333333333313</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="0"/>
@@ -50839,19 +50839,19 @@
       <c r="D22" s="7"/>
       <c r="E22" s="4">
         <f>SUM(E6:E20)</f>
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F22" s="4">
         <f>SUM(H6:H20)</f>
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G22" s="4">
         <f>SUM(I6:I20)</f>
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H22" s="4">
         <f>SUM(J6:J20)</f>
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I22" s="4">
         <f>SUM(K6:K20)</f>

</xml_diff>

<commit_message>
Tambah Slide 5 Aplikasi Game yang Kami Sarankan
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -108,12 +108,6 @@
     <t>Day 1</t>
   </si>
   <si>
-    <t>Story 4</t>
-  </si>
-  <si>
-    <t>Task 4.3</t>
-  </si>
-  <si>
     <t>Task 4.4</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>Kegunaan Benchmark</t>
+  </si>
+  <si>
+    <t>Beberapa Aplikasi Android yang kami sarankan</t>
+  </si>
+  <si>
+    <t>5 Aplikasi Games yang kami sarankan</t>
   </si>
 </sst>
 </file>
@@ -511,19 +511,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,25 +533,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="58211328"/>
-        <c:axId val="60351232"/>
+        <c:axId val="38279424"/>
+        <c:axId val="55071488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58211328"/>
+        <c:axId val="38279424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60351232"/>
+        <c:crossAx val="55071488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60351232"/>
+        <c:axId val="55071488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +559,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58211328"/>
+        <c:crossAx val="38279424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -572,7 +572,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -901,7 +901,7 @@
   <dimension ref="A1:XFD58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -917,7 +917,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -33690,7 +33690,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -50111,10 +50111,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
@@ -50154,13 +50154,13 @@
     <row r="6" spans="1:16384">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -50195,13 +50195,13 @@
     <row r="7" spans="1:16384">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
@@ -50236,13 +50236,13 @@
     <row r="8" spans="1:16384">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="4">
         <v>4</v>
@@ -50277,13 +50277,13 @@
     <row r="9" spans="1:16384">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4">
         <v>4</v>
@@ -50318,13 +50318,13 @@
     <row r="10" spans="1:16384">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4">
         <v>4</v>
@@ -50359,13 +50359,13 @@
     <row r="11" spans="1:16384">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="4">
         <v>6</v>
@@ -50400,13 +50400,13 @@
     <row r="12" spans="1:16384">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" s="4">
         <v>3</v>
@@ -50441,13 +50441,13 @@
     <row r="13" spans="1:16384">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4">
         <v>6</v>
@@ -50482,13 +50482,13 @@
     <row r="14" spans="1:16384">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="4">
         <v>6</v>
@@ -50523,13 +50523,13 @@
     <row r="15" spans="1:16384">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="4">
         <v>4</v>
@@ -50564,13 +50564,13 @@
     <row r="16" spans="1:16384">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -50605,13 +50605,13 @@
     <row r="17" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -50646,13 +50646,13 @@
     <row r="18" spans="1:21">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4">
         <v>10</v>
@@ -50687,13 +50687,13 @@
     <row r="19" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4">
         <v>8</v>
@@ -50728,13 +50728,13 @@
     <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" s="4">
         <v>9</v>
@@ -50769,7 +50769,7 @@
     <row r="21" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -50833,7 +50833,7 @@
     <row r="22" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -50842,24 +50842,24 @@
         <v>70</v>
       </c>
       <c r="F22" s="4">
+        <f>SUM(F6:F20)</f>
+        <v>64</v>
+      </c>
+      <c r="G22" s="4">
+        <f>SUM(G6:G20)</f>
+        <v>60</v>
+      </c>
+      <c r="H22" s="4">
         <f>SUM(H6:H20)</f>
         <v>51</v>
       </c>
-      <c r="G22" s="4">
+      <c r="I22" s="4">
         <f>SUM(I6:I20)</f>
         <v>46</v>
       </c>
-      <c r="H22" s="4">
+      <c r="J22" s="4">
         <f>SUM(J6:J20)</f>
         <v>39</v>
-      </c>
-      <c r="I22" s="4">
-        <f>SUM(K6:K20)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
-        <f>SUM(L6:L20)</f>
-        <v>0</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>

</xml_diff>

<commit_message>
Membuat slide 5 Aplikasi Utility
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -108,12 +108,6 @@
     <t>Day 1</t>
   </si>
   <si>
-    <t>Story 4</t>
-  </si>
-  <si>
-    <t>Task 4.3</t>
-  </si>
-  <si>
     <t>Task 4.4</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>Kegunaan Benchmark</t>
+  </si>
+  <si>
+    <t>Beberapa Aplikasi Android yang kami sarankan</t>
+  </si>
+  <si>
+    <t>5 Aplikasi Games yang kami sarankan</t>
   </si>
 </sst>
 </file>
@@ -511,19 +511,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,25 +533,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="58211328"/>
-        <c:axId val="60351232"/>
+        <c:axId val="38279424"/>
+        <c:axId val="55071488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58211328"/>
+        <c:axId val="38279424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60351232"/>
+        <c:crossAx val="55071488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60351232"/>
+        <c:axId val="55071488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +559,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58211328"/>
+        <c:crossAx val="38279424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -572,7 +572,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -901,7 +901,7 @@
   <dimension ref="A1:XFD58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -917,7 +917,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -33690,7 +33690,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -50111,10 +50111,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
@@ -50154,13 +50154,13 @@
     <row r="6" spans="1:16384">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -50195,13 +50195,13 @@
     <row r="7" spans="1:16384">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
@@ -50236,13 +50236,13 @@
     <row r="8" spans="1:16384">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="4">
         <v>4</v>
@@ -50277,13 +50277,13 @@
     <row r="9" spans="1:16384">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4">
         <v>4</v>
@@ -50318,13 +50318,13 @@
     <row r="10" spans="1:16384">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4">
         <v>4</v>
@@ -50359,13 +50359,13 @@
     <row r="11" spans="1:16384">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="4">
         <v>6</v>
@@ -50400,13 +50400,13 @@
     <row r="12" spans="1:16384">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" s="4">
         <v>3</v>
@@ -50441,13 +50441,13 @@
     <row r="13" spans="1:16384">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4">
         <v>6</v>
@@ -50482,13 +50482,13 @@
     <row r="14" spans="1:16384">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="4">
         <v>6</v>
@@ -50523,13 +50523,13 @@
     <row r="15" spans="1:16384">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="4">
         <v>4</v>
@@ -50564,13 +50564,13 @@
     <row r="16" spans="1:16384">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -50605,13 +50605,13 @@
     <row r="17" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -50646,13 +50646,13 @@
     <row r="18" spans="1:21">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4">
         <v>10</v>
@@ -50687,13 +50687,13 @@
     <row r="19" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4">
         <v>8</v>
@@ -50728,13 +50728,13 @@
     <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" s="4">
         <v>9</v>
@@ -50769,7 +50769,7 @@
     <row r="21" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -50833,7 +50833,7 @@
     <row r="22" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -50842,24 +50842,24 @@
         <v>70</v>
       </c>
       <c r="F22" s="4">
+        <f>SUM(F6:F20)</f>
+        <v>64</v>
+      </c>
+      <c r="G22" s="4">
+        <f>SUM(G6:G20)</f>
+        <v>60</v>
+      </c>
+      <c r="H22" s="4">
         <f>SUM(H6:H20)</f>
         <v>51</v>
       </c>
-      <c r="G22" s="4">
+      <c r="I22" s="4">
         <f>SUM(I6:I20)</f>
         <v>46</v>
       </c>
-      <c r="H22" s="4">
+      <c r="J22" s="4">
         <f>SUM(J6:J20)</f>
         <v>39</v>
-      </c>
-      <c r="I22" s="4">
-        <f>SUM(K6:K20)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
-        <f>SUM(L6:L20)</f>
-        <v>0</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>

</xml_diff>

<commit_message>
Edit Burn Down Chart & Logbook Day 6
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Project</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Day 1</t>
-  </si>
-  <si>
-    <t>Task 4.4</t>
   </si>
   <si>
     <t>Ideal - Remaining efforts in uninterrupted working hours</t>
@@ -187,6 +184,12 @@
   </si>
   <si>
     <t>5 Aplikasi Games yang kami sarankan</t>
+  </si>
+  <si>
+    <t>5 Aplikasi Utility yang kami sarankan</t>
+  </si>
+  <si>
+    <t>5 Aplikasi Sosial Media yang kami sarankan</t>
   </si>
 </sst>
 </file>
@@ -407,42 +410,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$21:$Q$21</c:f>
+              <c:f>Sheet1!$F$22:$Q$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>64.166666666666671</c:v>
+                  <c:v>67.833333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58.333333333333336</c:v>
+                  <c:v>61.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.5</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.666666666666664</c:v>
+                  <c:v>49.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.833333333333329</c:v>
+                  <c:v>43.166666666666671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.999999999999993</c:v>
+                  <c:v>37.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.166666666666661</c:v>
+                  <c:v>30.833333333333339</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.333333333333329</c:v>
+                  <c:v>24.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.499999999999996</c:v>
+                  <c:v>18.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.666666666666664</c:v>
+                  <c:v>12.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.8333333333333313</c:v>
+                  <c:v>6.1666666666666687</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -506,24 +509,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$Q$22</c:f>
+              <c:f>Sheet1!$F$23:$Q$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,25 +536,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="38279424"/>
-        <c:axId val="55071488"/>
+        <c:axId val="46349312"/>
+        <c:axId val="64680704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38279424"/>
+        <c:axId val="46349312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55071488"/>
+        <c:crossAx val="64680704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55071488"/>
+        <c:axId val="64680704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +562,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38279424"/>
+        <c:crossAx val="46349312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -572,7 +575,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -584,13 +587,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>846668</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>148165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>74084</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>137582</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -898,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD58"/>
+  <dimension ref="A1:XFD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -917,7 +920,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -33690,7 +33693,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -50111,10 +50114,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
@@ -50154,13 +50157,13 @@
     <row r="6" spans="1:16384">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -50195,13 +50198,13 @@
     <row r="7" spans="1:16384">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
@@ -50236,13 +50239,13 @@
     <row r="8" spans="1:16384">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="4">
         <v>4</v>
@@ -50277,13 +50280,13 @@
     <row r="9" spans="1:16384">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4">
         <v>4</v>
@@ -50318,13 +50321,13 @@
     <row r="10" spans="1:16384">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="4">
         <v>4</v>
@@ -50359,13 +50362,13 @@
     <row r="11" spans="1:16384">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4">
         <v>6</v>
@@ -50400,13 +50403,13 @@
     <row r="12" spans="1:16384">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="4">
         <v>3</v>
@@ -50441,13 +50444,13 @@
     <row r="13" spans="1:16384">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="4">
         <v>6</v>
@@ -50482,13 +50485,13 @@
     <row r="14" spans="1:16384">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4">
         <v>6</v>
@@ -50523,13 +50526,13 @@
     <row r="15" spans="1:16384">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="4">
         <v>4</v>
@@ -50564,13 +50567,13 @@
     <row r="16" spans="1:16384">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -50605,13 +50608,13 @@
     <row r="17" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -50646,13 +50649,13 @@
     <row r="18" spans="1:21">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="4">
         <v>10</v>
@@ -50687,13 +50690,13 @@
     <row r="19" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="4">
         <v>8</v>
@@ -50728,31 +50731,31 @@
     <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="E20" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F20" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G20" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H20" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I20" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J20" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -50768,63 +50771,40 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="1"/>
-      <c r="B21" s="7" t="s">
-        <v>15</v>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="C21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E21" s="4">
-        <f>SUM(E6:E20)</f>
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="F21" s="4">
-        <f>E21-$E$21/12</f>
-        <v>64.166666666666671</v>
+        <v>9</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" ref="G21:Q21" si="0">F21-$E$21/12</f>
-        <v>58.333333333333336</v>
+        <v>9</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>9</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="0"/>
-        <v>46.666666666666664</v>
+        <v>9</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="0"/>
-        <v>40.833333333333329</v>
+        <v>9</v>
       </c>
-      <c r="K21" s="4">
-        <f t="shared" si="0"/>
-        <v>34.999999999999993</v>
-      </c>
-      <c r="L21" s="4">
-        <f t="shared" si="0"/>
-        <v>29.166666666666661</v>
-      </c>
-      <c r="M21" s="4">
-        <f t="shared" si="0"/>
-        <v>23.333333333333329</v>
-      </c>
-      <c r="N21" s="4">
-        <f>M21-$E$21/12</f>
-        <v>17.499999999999996</v>
-      </c>
-      <c r="O21" s="4">
-        <f t="shared" si="0"/>
-        <v>11.666666666666664</v>
-      </c>
-      <c r="P21" s="4">
-        <f t="shared" si="0"/>
-        <v>5.8333333333333313</v>
-      </c>
-      <c r="Q21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -50833,41 +50813,62 @@
     <row r="22" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="4">
-        <f>SUM(E6:E20)</f>
-        <v>70</v>
+        <f>SUM(E6:E21)</f>
+        <v>74</v>
       </c>
       <c r="F22" s="4">
-        <f>SUM(F6:F20)</f>
-        <v>64</v>
+        <f>E22-$E$22/12</f>
+        <v>67.833333333333329</v>
       </c>
       <c r="G22" s="4">
-        <f>SUM(G6:G20)</f>
-        <v>60</v>
+        <f t="shared" ref="G22:Q22" si="0">F22-$E$22/12</f>
+        <v>61.666666666666664</v>
       </c>
       <c r="H22" s="4">
-        <f>SUM(H6:H20)</f>
-        <v>51</v>
+        <f t="shared" si="0"/>
+        <v>55.5</v>
       </c>
       <c r="I22" s="4">
-        <f>SUM(I6:I20)</f>
-        <v>46</v>
+        <f t="shared" si="0"/>
+        <v>49.333333333333336</v>
       </c>
       <c r="J22" s="4">
-        <f>SUM(J6:J20)</f>
-        <v>39</v>
+        <f t="shared" si="0"/>
+        <v>43.166666666666671</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
+      <c r="K22" s="4">
+        <f t="shared" si="0"/>
+        <v>37.000000000000007</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="0"/>
+        <v>30.833333333333339</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" si="0"/>
+        <v>24.666666666666671</v>
+      </c>
+      <c r="N22" s="4">
+        <f>M22-$E$22/12</f>
+        <v>18.500000000000004</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="0"/>
+        <v>12.333333333333336</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="0"/>
+        <v>6.1666666666666687</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -50875,22 +50876,42 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="B23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="4">
+        <f>SUM(E6:E21)</f>
+        <v>74</v>
+      </c>
+      <c r="F23" s="4">
+        <f>SUM(F6:F21)</f>
+        <v>68</v>
+      </c>
+      <c r="G23" s="4">
+        <f>SUM(G6:G21)</f>
+        <v>64</v>
+      </c>
+      <c r="H23" s="4">
+        <f>SUM(H6:H21)</f>
+        <v>55</v>
+      </c>
+      <c r="I23" s="4">
+        <f>SUM(I6:I21)</f>
+        <v>50</v>
+      </c>
+      <c r="J23" s="4">
+        <f>SUM(J6:J21)</f>
+        <v>43</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -51701,11 +51722,34 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
     </row>
+    <row r="59" spans="1:21">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+    </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="D3:K3"/>
     <mergeCell ref="E1:J1"/>
   </mergeCells>

</xml_diff>

<commit_message>
update logbook dan burndown chart
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
   <si>
     <t>Project</t>
   </si>
@@ -190,6 +190,27 @@
   </si>
   <si>
     <t>5 Aplikasi Sosial Media yang kami sarankan</t>
+  </si>
+  <si>
+    <t>Re-Checking, Re-Correct, Re-Designing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meringkas/menghapus topik Pengenalan Android </t>
+  </si>
+  <si>
+    <t>Meringkas/menghapus topik Trik Android</t>
+  </si>
+  <si>
+    <t>Meringkas/menghapus topik  Masalah di Android</t>
+  </si>
+  <si>
+    <t>Meringkas/menghapus topik Benchmark</t>
+  </si>
+  <si>
+    <t>Meringkas/menghapus topik Aplikasi Android yang Disarankan</t>
+  </si>
+  <si>
+    <t>Meringkas/menghapus topik Android Google Play</t>
   </si>
 </sst>
 </file>
@@ -340,7 +361,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr lang="en-US"/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -362,6 +383,16 @@
             <c:v>Ideal burndown</c:v>
           </c:tx>
           <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
@@ -410,42 +441,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$Q$22</c:f>
+              <c:f>Sheet1!$F$32:$Q$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>67.833333333333329</c:v>
+                  <c:v>70.583333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61.666666666666664</c:v>
+                  <c:v>64.166666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.5</c:v>
+                  <c:v>57.749999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.333333333333336</c:v>
+                  <c:v>51.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.166666666666671</c:v>
+                  <c:v>44.916666666666664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.000000000000007</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.833333333333339</c:v>
+                  <c:v>32.083333333333336</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.666666666666671</c:v>
+                  <c:v>25.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.500000000000004</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.333333333333336</c:v>
+                  <c:v>12.833333333333332</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.1666666666666687</c:v>
+                  <c:v>6.4166666666666652</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -461,6 +492,16 @@
             <c:v>Actual burndown</c:v>
           </c:tx>
           <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
@@ -509,7 +550,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$23:$Q$23</c:f>
+              <c:f>Sheet1!$F$33:$Q$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -536,25 +577,35 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="46349312"/>
-        <c:axId val="64680704"/>
+        <c:axId val="55411072"/>
+        <c:axId val="55412608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46349312"/>
+        <c:axId val="55411072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64680704"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="55412608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64680704"/>
+        <c:axId val="55412608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +613,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46349312"/>
+        <c:crossAx val="55411072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -570,12 +621,22 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -587,13 +648,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>846668</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>148165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>74084</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>137582</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -901,16 +962,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD59"/>
+  <dimension ref="A1:XFD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -50183,7 +50244,9 @@
       <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -50224,7 +50287,9 @@
       <c r="J7" s="4">
         <v>0</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -50265,7 +50330,9 @@
       <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -50306,7 +50373,9 @@
       <c r="J9" s="4">
         <v>0</v>
       </c>
-      <c r="K9" s="4"/>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -50347,7 +50416,9 @@
       <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="4"/>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -50388,7 +50459,9 @@
       <c r="J11" s="4">
         <v>0</v>
       </c>
-      <c r="K11" s="4"/>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -50429,7 +50502,9 @@
       <c r="J12" s="4">
         <v>0</v>
       </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -50470,7 +50545,9 @@
       <c r="J13" s="4">
         <v>0</v>
       </c>
-      <c r="K13" s="4"/>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -50511,7 +50588,9 @@
       <c r="J14" s="4">
         <v>6</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -50552,7 +50631,9 @@
       <c r="J15" s="4">
         <v>4</v>
       </c>
-      <c r="K15" s="4"/>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -50593,7 +50674,9 @@
       <c r="J16" s="4">
         <v>1</v>
       </c>
-      <c r="K16" s="4"/>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -50634,7 +50717,9 @@
       <c r="J17" s="4">
         <v>1</v>
       </c>
-      <c r="K17" s="4"/>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -50675,7 +50760,9 @@
       <c r="J18" s="4">
         <v>10</v>
       </c>
-      <c r="K18" s="4"/>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -50716,7 +50803,9 @@
       <c r="J19" s="4">
         <v>8</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -50757,7 +50846,9 @@
       <c r="J20" s="4">
         <v>4</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -50798,7 +50889,9 @@
       <c r="J21" s="4">
         <v>9</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -50812,63 +50905,42 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="1"/>
-      <c r="B22" s="7" t="s">
-        <v>14</v>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="C22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E22" s="4">
-        <f>SUM(E6:E21)</f>
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F22" s="4">
-        <f>E22-$E$22/12</f>
-        <v>67.833333333333329</v>
+        <v>3</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" ref="G22:Q22" si="0">F22-$E$22/12</f>
-        <v>61.666666666666664</v>
+        <v>3</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="0"/>
-        <v>55.5</v>
+        <v>3</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="0"/>
-        <v>49.333333333333336</v>
+        <v>3</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="0"/>
-        <v>43.166666666666671</v>
+        <v>3</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="0"/>
-        <v>37.000000000000007</v>
+        <v>3</v>
       </c>
-      <c r="L22" s="4">
-        <f t="shared" si="0"/>
-        <v>30.833333333333339</v>
-      </c>
-      <c r="M22" s="4">
-        <f t="shared" si="0"/>
-        <v>24.666666666666671</v>
-      </c>
-      <c r="N22" s="4">
-        <f>M22-$E$22/12</f>
-        <v>18.500000000000004</v>
-      </c>
-      <c r="O22" s="4">
-        <f t="shared" si="0"/>
-        <v>12.333333333333336</v>
-      </c>
-      <c r="P22" s="4">
-        <f t="shared" si="0"/>
-        <v>6.1666666666666687</v>
-      </c>
-      <c r="Q22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -50876,35 +50948,21 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="1"/>
-      <c r="B23" s="7" t="s">
-        <v>15</v>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="4">
-        <f>SUM(E6:E21)</f>
-        <v>74</v>
+      <c r="C23" s="3" t="s">
+        <v>42</v>
       </c>
-      <c r="F23" s="4">
-        <f>SUM(F6:F21)</f>
-        <v>68</v>
+      <c r="D23" s="3" t="s">
+        <v>44</v>
       </c>
-      <c r="G23" s="4">
-        <f>SUM(G6:G21)</f>
-        <v>64</v>
-      </c>
-      <c r="H23" s="4">
-        <f>SUM(H6:H21)</f>
-        <v>55</v>
-      </c>
-      <c r="I23" s="4">
-        <f>SUM(I6:I21)</f>
-        <v>50</v>
-      </c>
-      <c r="J23" s="4">
-        <f>SUM(J6:J21)</f>
-        <v>43</v>
-      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -50919,22 +50977,42 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2</v>
+      </c>
+      <c r="F24" s="4">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>2</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>2</v>
+      </c>
+      <c r="J24" s="4">
+        <v>2</v>
+      </c>
+      <c r="K24" s="4">
+        <v>2</v>
+      </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -50942,22 +51020,28 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="B25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
@@ -50965,22 +51049,28 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -50988,22 +51078,42 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2</v>
+      </c>
+      <c r="F27" s="4">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4">
+        <v>2</v>
+      </c>
+      <c r="H27" s="4">
+        <v>2</v>
+      </c>
+      <c r="I27" s="4">
+        <v>2</v>
+      </c>
+      <c r="J27" s="4">
+        <v>2</v>
+      </c>
+      <c r="K27" s="4">
+        <v>2</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
@@ -51011,22 +51121,24 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+      <c r="B28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -51034,22 +51146,24 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+      <c r="B29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
@@ -51057,22 +51171,24 @@
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
+      <c r="B30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
@@ -51080,22 +51196,24 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
+      <c r="B31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
@@ -51103,22 +51221,63 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="B32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="4">
+        <f>SUM(E6:E22)</f>
+        <v>77</v>
+      </c>
+      <c r="F32" s="4">
+        <f>E32-$E$32/12</f>
+        <v>70.583333333333329</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" ref="G32:Q32" si="0">F32-$E$32/12</f>
+        <v>64.166666666666657</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="0"/>
+        <v>57.749999999999993</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="0"/>
+        <v>51.333333333333329</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="0"/>
+        <v>44.916666666666664</v>
+      </c>
+      <c r="K32" s="4">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+      <c r="L32" s="4">
+        <f t="shared" si="0"/>
+        <v>32.083333333333336</v>
+      </c>
+      <c r="M32" s="4">
+        <f t="shared" si="0"/>
+        <v>25.666666666666668</v>
+      </c>
+      <c r="N32" s="4">
+        <f>M32-$E$32/12</f>
+        <v>19.25</v>
+      </c>
+      <c r="O32" s="4">
+        <f t="shared" si="0"/>
+        <v>12.833333333333332</v>
+      </c>
+      <c r="P32" s="4">
+        <f t="shared" si="0"/>
+        <v>6.4166666666666652</v>
+      </c>
+      <c r="Q32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -51126,22 +51285,42 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
+      <c r="B33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="4">
+        <f>SUM(E6:E22)</f>
+        <v>77</v>
+      </c>
+      <c r="F33" s="4">
+        <f>SUM(F6:F21)</f>
+        <v>68</v>
+      </c>
+      <c r="G33" s="4">
+        <f>SUM(G6:G21)</f>
+        <v>64</v>
+      </c>
+      <c r="H33" s="4">
+        <f>SUM(H6:H21)</f>
+        <v>55</v>
+      </c>
+      <c r="I33" s="4">
+        <f>SUM(I6:I21)</f>
+        <v>50</v>
+      </c>
+      <c r="J33" s="4">
+        <f>SUM(J6:J21)</f>
+        <v>43</v>
+      </c>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -51745,11 +51924,241 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
     </row>
+    <row r="60" spans="1:21">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+    </row>
+    <row r="65" spans="1:21">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+    </row>
+    <row r="66" spans="1:21">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+    </row>
+    <row r="67" spans="1:21">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+    </row>
+    <row r="68" spans="1:21">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+    </row>
+    <row r="69" spans="1:21">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+    </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="D3:K3"/>
     <mergeCell ref="E1:J1"/>
   </mergeCells>

</xml_diff>

<commit_message>
update burndown chart dan logbook
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>Project</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Meringkas/menghapus topik Android Google Play</t>
+  </si>
+  <si>
+    <t>Jenis-jenis Layar</t>
+  </si>
+  <si>
+    <t>Tips Memilih Layar</t>
   </si>
 </sst>
 </file>
@@ -555,19 +561,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -577,11 +589,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="55411072"/>
-        <c:axId val="55412608"/>
+        <c:axId val="51347840"/>
+        <c:axId val="51349376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55411072"/>
+        <c:axId val="51347840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,14 +610,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55412608"/>
+        <c:crossAx val="51349376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55412608"/>
+        <c:axId val="51349376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +625,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55411072"/>
+        <c:crossAx val="51347840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -636,7 +648,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -964,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:K27"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50247,7 +50259,9 @@
       <c r="K6" s="4">
         <v>0</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -50290,7 +50304,9 @@
       <c r="K7" s="4">
         <v>0</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -50333,7 +50349,9 @@
       <c r="K8" s="4">
         <v>0</v>
       </c>
-      <c r="L8" s="4"/>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -50376,7 +50394,9 @@
       <c r="K9" s="4">
         <v>0</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -50419,7 +50439,9 @@
       <c r="K10" s="4">
         <v>0</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -50462,7 +50484,9 @@
       <c r="K11" s="4">
         <v>0</v>
       </c>
-      <c r="L11" s="4"/>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -50505,7 +50529,9 @@
       <c r="K12" s="4">
         <v>0</v>
       </c>
-      <c r="L12" s="4"/>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -50548,7 +50574,9 @@
       <c r="K13" s="4">
         <v>0</v>
       </c>
-      <c r="L13" s="4"/>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -50591,7 +50619,9 @@
       <c r="K14" s="4">
         <v>0</v>
       </c>
-      <c r="L14" s="4"/>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -50634,7 +50664,9 @@
       <c r="K15" s="4">
         <v>0</v>
       </c>
-      <c r="L15" s="4"/>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -50677,7 +50709,9 @@
       <c r="K16" s="4">
         <v>0</v>
       </c>
-      <c r="L16" s="4"/>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -50720,7 +50754,9 @@
       <c r="K17" s="4">
         <v>0</v>
       </c>
-      <c r="L17" s="4"/>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -50763,7 +50799,9 @@
       <c r="K18" s="4">
         <v>0</v>
       </c>
-      <c r="L18" s="4"/>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -50806,7 +50844,9 @@
       <c r="K19" s="4">
         <v>0</v>
       </c>
-      <c r="L19" s="4"/>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -50849,7 +50889,9 @@
       <c r="K20" s="4">
         <v>0</v>
       </c>
-      <c r="L20" s="4"/>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -50892,7 +50934,9 @@
       <c r="K21" s="4">
         <v>0</v>
       </c>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -50915,27 +50959,29 @@
         <v>43</v>
       </c>
       <c r="E22" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G22" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I22" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J22" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K22" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -50987,27 +51033,29 @@
         <v>45</v>
       </c>
       <c r="E24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="L24" s="4"/>
+      <c r="L24" s="4">
+        <v>0</v>
+      </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -51029,14 +51077,30 @@
       <c r="D25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0</v>
+      </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -51058,14 +51122,30 @@
       <c r="D26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0</v>
+      </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
@@ -51088,27 +51168,29 @@
         <v>48</v>
       </c>
       <c r="E27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="L27" s="4"/>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -51124,16 +51206,36 @@
       <c r="B28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
+      <c r="C28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2</v>
+      </c>
+      <c r="G28" s="4">
+        <v>2</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>2</v>
+      </c>
+      <c r="J28" s="4">
+        <v>2</v>
+      </c>
+      <c r="K28" s="4">
+        <v>2</v>
+      </c>
+      <c r="L28" s="4">
+        <v>2</v>
+      </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -51149,16 +51251,36 @@
       <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
+      <c r="C29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1</v>
+      </c>
+      <c r="J29" s="4">
+        <v>1</v>
+      </c>
+      <c r="K29" s="4">
+        <v>1</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1</v>
+      </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -51227,7 +51349,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="4">
-        <f>SUM(E6:E22)</f>
+        <f>SUM(E6:E31)</f>
         <v>77</v>
       </c>
       <c r="F32" s="4">
@@ -51239,7 +51361,7 @@
         <v>64.166666666666657</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="0"/>
+        <f>G32-$E$32/12</f>
         <v>57.749999999999993</v>
       </c>
       <c r="I32" s="4">
@@ -51291,31 +51413,37 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="4">
-        <f>SUM(E6:E22)</f>
+        <f>SUM(E6:E31)</f>
         <v>77</v>
       </c>
       <c r="F33" s="4">
-        <f>SUM(F6:F21)</f>
-        <v>68</v>
+        <f>SUM(F6:F31)</f>
+        <v>71</v>
       </c>
       <c r="G33" s="4">
-        <f>SUM(G6:G21)</f>
-        <v>64</v>
+        <f>SUM(G6:G31)</f>
+        <v>67</v>
       </c>
       <c r="H33" s="4">
-        <f>SUM(H6:H21)</f>
-        <v>55</v>
+        <f>SUM(H6:H31)</f>
+        <v>58</v>
       </c>
       <c r="I33" s="4">
-        <f>SUM(I6:I21)</f>
-        <v>50</v>
+        <f>SUM(I6:I31)</f>
+        <v>53</v>
       </c>
       <c r="J33" s="4">
-        <f>SUM(J6:J21)</f>
-        <v>43</v>
+        <f>SUM(J6:J31)</f>
+        <v>46</v>
       </c>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
+      <c r="K33" s="4">
+        <f>SUM(K6:K31)</f>
+        <v>3</v>
+      </c>
+      <c r="L33" s="4">
+        <f>SUM(L6:L31)</f>
+        <v>3</v>
+      </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>

</xml_diff>

<commit_message>
update logbook & burndownchart
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -581,6 +581,21 @@
                 <c:pt idx="6">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -589,11 +604,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="51347840"/>
-        <c:axId val="51349376"/>
+        <c:axId val="56852864"/>
+        <c:axId val="56854400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51347840"/>
+        <c:axId val="56852864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,14 +625,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51349376"/>
+        <c:crossAx val="56854400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51349376"/>
+        <c:axId val="56854400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +640,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51347840"/>
+        <c:crossAx val="56852864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -648,7 +663,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -976,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51003,14 +51018,30 @@
       <c r="D23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -51413,42 +51444,57 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="4">
-        <f>SUM(E6:E31)</f>
+        <f t="shared" ref="E33:L33" si="1">SUM(E6:E31)</f>
         <v>77</v>
       </c>
       <c r="F33" s="4">
-        <f>SUM(F6:F31)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="G33" s="4">
-        <f>SUM(G6:G31)</f>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="H33" s="4">
-        <f>SUM(H6:H31)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="I33" s="4">
-        <f>SUM(I6:I31)</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="J33" s="4">
-        <f>SUM(J6:J31)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="K33" s="4">
-        <f>SUM(K6:K31)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L33" s="4">
-        <f>SUM(L6:L31)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
+      <c r="M33" s="4">
+        <f>SUM(M6:M31)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="4">
+        <f>SUM(N6:N31)</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="4">
+        <f>SUM(O6:O31)</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="4">
+        <f>SUM(P6:P31)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="4">
+        <f>SUM(Q6:Q31)</f>
+        <v>0</v>
+      </c>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>

</xml_diff>

<commit_message>
update burndown chart & logbook
</commit_message>
<xml_diff>
--- a/public/BurnDownChart.xlsx
+++ b/public/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="56">
   <si>
     <t>Project</t>
   </si>
@@ -217,6 +217,21 @@
   </si>
   <si>
     <t>Tips Memilih Layar</t>
+  </si>
+  <si>
+    <t>Tips Perawatan Fisik pada Baterai Android</t>
+  </si>
+  <si>
+    <t>Edit Style Slide</t>
+  </si>
+  <si>
+    <t>Tips agar Perangkat Android tidak Lelet</t>
+  </si>
+  <si>
+    <t>Tips</t>
+  </si>
+  <si>
+    <t>Tips Memilih Perangkat Android yang Asli atau Replika</t>
   </si>
 </sst>
 </file>
@@ -447,45 +462,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$32:$Q$32</c:f>
+              <c:f>Sheet1!$F$45:$Q$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>70.583333333333329</c:v>
+                  <c:v>84.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.166666666666657</c:v>
+                  <c:v>76.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.749999999999993</c:v>
+                  <c:v>68.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.333333333333329</c:v>
+                  <c:v>61.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.916666666666664</c:v>
+                  <c:v>53.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.5</c:v>
+                  <c:v>45.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.083333333333336</c:v>
+                  <c:v>38.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.666666666666668</c:v>
+                  <c:v>30.666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.25</c:v>
+                  <c:v>22.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.833333333333332</c:v>
+                  <c:v>15.333333333333325</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.4166666666666652</c:v>
+                  <c:v>7.6666666666666581</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>-8.8817841970012523E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,33 +571,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$33:$Q$33</c:f>
+              <c:f>Sheet1!$F$46:$Q$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>71</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -604,11 +619,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="56852864"/>
-        <c:axId val="56854400"/>
+        <c:axId val="57377152"/>
+        <c:axId val="57378688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56852864"/>
+        <c:axId val="57377152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,14 +640,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56854400"/>
+        <c:crossAx val="57378688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56854400"/>
+        <c:axId val="57378688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,7 +655,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56852864"/>
+        <c:crossAx val="57377152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -663,7 +678,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -675,13 +690,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>846668</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>148165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>74084</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>137582</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -989,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD69"/>
+  <dimension ref="A1:XFD82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50277,7 +50292,9 @@
       <c r="L6" s="4">
         <v>0</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -50322,7 +50339,9 @@
       <c r="L7" s="4">
         <v>0</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
@@ -50367,7 +50386,9 @@
       <c r="L8" s="4">
         <v>0</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -50412,7 +50433,9 @@
       <c r="L9" s="4">
         <v>0</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -50457,7 +50480,9 @@
       <c r="L10" s="4">
         <v>0</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -50502,7 +50527,9 @@
       <c r="L11" s="4">
         <v>0</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -50547,7 +50574,9 @@
       <c r="L12" s="4">
         <v>0</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -50592,7 +50621,9 @@
       <c r="L13" s="4">
         <v>0</v>
       </c>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -50637,7 +50668,9 @@
       <c r="L14" s="4">
         <v>0</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -50682,7 +50715,9 @@
       <c r="L15" s="4">
         <v>0</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -50727,7 +50762,9 @@
       <c r="L16" s="4">
         <v>0</v>
       </c>
-      <c r="M16" s="4"/>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -50772,7 +50809,9 @@
       <c r="L17" s="4">
         <v>0</v>
       </c>
-      <c r="M17" s="4"/>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -50817,7 +50856,9 @@
       <c r="L18" s="4">
         <v>0</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -50862,7 +50903,9 @@
       <c r="L19" s="4">
         <v>0</v>
       </c>
-      <c r="M19" s="4"/>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -50907,7 +50950,9 @@
       <c r="L20" s="4">
         <v>0</v>
       </c>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -50952,7 +50997,9 @@
       <c r="L21" s="4">
         <v>0</v>
       </c>
-      <c r="M21" s="4"/>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -50974,30 +51021,32 @@
         <v>43</v>
       </c>
       <c r="E22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4">
+        <v>1</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -51019,30 +51068,32 @@
         <v>44</v>
       </c>
       <c r="E23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
-      <c r="M23" s="4"/>
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -51064,30 +51115,32 @@
         <v>45</v>
       </c>
       <c r="E24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4">
+        <v>1</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -51109,30 +51162,32 @@
         <v>46</v>
       </c>
       <c r="E25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="M25" s="4">
+        <v>1</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -51154,30 +51209,32 @@
         <v>47</v>
       </c>
       <c r="E26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
-      <c r="M26" s="4"/>
+      <c r="M26" s="4">
+        <v>1</v>
+      </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -51199,30 +51256,32 @@
         <v>48</v>
       </c>
       <c r="E27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
-      <c r="M27" s="4"/>
+      <c r="M27" s="4">
+        <v>1</v>
+      </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -51267,7 +51326,9 @@
       <c r="L28" s="4">
         <v>2</v>
       </c>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4">
+        <v>2</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
@@ -51312,7 +51373,9 @@
       <c r="L29" s="4">
         <v>1</v>
       </c>
-      <c r="M29" s="4"/>
+      <c r="M29" s="4">
+        <v>1</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
@@ -51327,17 +51390,39 @@
       <c r="B30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="C30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3</v>
+      </c>
+      <c r="H30" s="4">
+        <v>3</v>
+      </c>
+      <c r="I30" s="4">
+        <v>3</v>
+      </c>
+      <c r="J30" s="4">
+        <v>3</v>
+      </c>
+      <c r="K30" s="4">
+        <v>3</v>
+      </c>
+      <c r="L30" s="4">
+        <v>3</v>
+      </c>
+      <c r="M30" s="4">
+        <v>3</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
@@ -51352,17 +51437,39 @@
       <c r="B31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="C31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1</v>
+      </c>
+      <c r="M31" s="4">
+        <v>1</v>
+      </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
@@ -51374,63 +51481,46 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="1"/>
-      <c r="B32" s="7" t="s">
-        <v>14</v>
+      <c r="B32" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="C32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E32" s="4">
-        <f>SUM(E6:E31)</f>
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="F32" s="4">
-        <f>E32-$E$32/12</f>
-        <v>70.583333333333329</v>
+        <v>2</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" ref="G32:Q32" si="0">F32-$E$32/12</f>
-        <v>64.166666666666657</v>
+        <v>2</v>
       </c>
       <c r="H32" s="4">
-        <f>G32-$E$32/12</f>
-        <v>57.749999999999993</v>
+        <v>2</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="0"/>
-        <v>51.333333333333329</v>
+        <v>2</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="0"/>
-        <v>44.916666666666664</v>
+        <v>2</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="0"/>
-        <v>38.5</v>
+        <v>2</v>
       </c>
       <c r="L32" s="4">
-        <f t="shared" si="0"/>
-        <v>32.083333333333336</v>
+        <v>2</v>
       </c>
       <c r="M32" s="4">
-        <f t="shared" si="0"/>
-        <v>25.666666666666668</v>
+        <v>2</v>
       </c>
-      <c r="N32" s="4">
-        <f>M32-$E$32/12</f>
-        <v>19.25</v>
-      </c>
-      <c r="O32" s="4">
-        <f t="shared" si="0"/>
-        <v>12.833333333333332</v>
-      </c>
-      <c r="P32" s="4">
-        <f t="shared" si="0"/>
-        <v>6.4166666666666652</v>
-      </c>
-      <c r="Q32" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -51438,63 +51528,46 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="1"/>
-      <c r="B33" s="7" t="s">
-        <v>15</v>
+      <c r="B33" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="C33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E33" s="4">
-        <f t="shared" ref="E33:L33" si="1">SUM(E6:E31)</f>
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="1"/>
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="1"/>
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="1"/>
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="1"/>
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="J33" s="4">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L33" s="4">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M33" s="4">
-        <f>SUM(M6:M31)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
-      <c r="N33" s="4">
-        <f>SUM(N6:N31)</f>
-        <v>0</v>
-      </c>
-      <c r="O33" s="4">
-        <f>SUM(O6:O31)</f>
-        <v>0</v>
-      </c>
-      <c r="P33" s="4">
-        <f>SUM(P6:P31)</f>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="4">
-        <f>SUM(Q6:Q31)</f>
-        <v>0</v>
-      </c>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -51502,22 +51575,24 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
+      <c r="B34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
@@ -51525,22 +51600,24 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="B35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
@@ -51548,22 +51625,24 @@
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="B36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
@@ -51571,22 +51650,24 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
+      <c r="B37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
@@ -51594,22 +51675,24 @@
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
+      <c r="B38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
@@ -51617,22 +51700,24 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
+      <c r="B39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
@@ -51640,22 +51725,24 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
+      <c r="B40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -51663,22 +51750,24 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="B41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
@@ -51686,22 +51775,24 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
+      <c r="B42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
@@ -51709,22 +51800,24 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
+      <c r="B43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
@@ -51732,22 +51825,24 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
+      <c r="B44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
@@ -51755,22 +51850,63 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
+      <c r="B45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="4">
+        <f>SUM(E6:E33)</f>
+        <v>92</v>
+      </c>
+      <c r="F45" s="4">
+        <f>E45-$E$45/12</f>
+        <v>84.333333333333329</v>
+      </c>
+      <c r="G45" s="4">
+        <f t="shared" ref="G45:Q45" si="0">F45-$E$45/12</f>
+        <v>76.666666666666657</v>
+      </c>
+      <c r="H45" s="4">
+        <f>G45-$E$45/12</f>
+        <v>68.999999999999986</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" si="0"/>
+        <v>61.333333333333321</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" si="0"/>
+        <v>53.666666666666657</v>
+      </c>
+      <c r="K45" s="4">
+        <f t="shared" si="0"/>
+        <v>45.999999999999993</v>
+      </c>
+      <c r="L45" s="4">
+        <f t="shared" si="0"/>
+        <v>38.333333333333329</v>
+      </c>
+      <c r="M45" s="4">
+        <f t="shared" si="0"/>
+        <v>30.666666666666661</v>
+      </c>
+      <c r="N45" s="4">
+        <f>M45-$E$45/12</f>
+        <v>22.999999999999993</v>
+      </c>
+      <c r="O45" s="4">
+        <f t="shared" si="0"/>
+        <v>15.333333333333325</v>
+      </c>
+      <c r="P45" s="4">
+        <f t="shared" si="0"/>
+        <v>7.6666666666666581</v>
+      </c>
+      <c r="Q45" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.8817841970012523E-15</v>
+      </c>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
@@ -51778,22 +51914,63 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
+      <c r="B46" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="4">
+        <f t="shared" ref="E46:Q46" si="1">SUM(E6:E44)</f>
+        <v>92</v>
+      </c>
+      <c r="F46" s="4">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="K46" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="L46" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="M46" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="N46" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O46" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
@@ -52328,11 +52505,310 @@
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
     </row>
+    <row r="70" spans="1:21">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+    </row>
+    <row r="71" spans="1:21">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+    </row>
+    <row r="72" spans="1:21">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+    </row>
+    <row r="73" spans="1:21">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+    </row>
+    <row r="74" spans="1:21">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+    </row>
+    <row r="75" spans="1:21">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+    </row>
+    <row r="76" spans="1:21">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+    </row>
+    <row r="77" spans="1:21">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+    </row>
+    <row r="78" spans="1:21">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+    </row>
+    <row r="79" spans="1:21">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+    </row>
+    <row r="80" spans="1:21">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+    </row>
+    <row r="81" spans="1:21">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+    </row>
+    <row r="82" spans="1:21">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+    </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
     <mergeCell ref="D3:K3"/>
     <mergeCell ref="E1:J1"/>
   </mergeCells>

</xml_diff>